<commit_message>
POC catalog PR Create Done
</commit_message>
<xml_diff>
--- a/GePS-YIL/Downloads/ExportItems.xlsx
+++ b/GePS-YIL/Downloads/ExportItems.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
   <si>
     <t xml:space="preserve">Sl. no.</t>
   </si>
@@ -54,12 +54,6 @@
   </si>
   <si>
     <t xml:space="preserve">Remarks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SO Item Number</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SVO Item Number</t>
   </si>
   <si>
     <t xml:space="preserve">RC-00027</t>
@@ -179,7 +173,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1:R3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="1" showOutlineSymbols="1" defaultGridColor="1" colorId="64" zoomScale="100" workbookViewId="0"/>
   </sheetViews>
@@ -228,40 +222,34 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>2</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0">
         <v>175.32</v>
       </c>
       <c r="F2" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="G2" t="s" s="0">
+      <c r="I2" t="s" s="0">
         <v>27</v>
-      </c>
-      <c r="H2" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I2" t="s" s="0">
-        <v>29</v>
       </c>
       <c r="J2" s="0">
         <v>21</v>
@@ -273,19 +261,10 @@
         <v>3.0</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>36</v>
-      </c>
-      <c r="O2" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>23</v>
-      </c>
-      <c r="R2" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3">
@@ -293,28 +272,28 @@
         <v>3</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E3" s="0">
         <v>185.32</v>
       </c>
       <c r="F3" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="G3" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="G3" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H3" t="s" s="0">
-        <v>34</v>
-      </c>
       <c r="I3" t="s" s="0">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="J3" s="0">
         <v>11</v>
@@ -326,19 +305,10 @@
         <v>5.0</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="O3" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>23</v>
-      </c>
-      <c r="R3" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>